<commit_message>
Updates spreadsheet with performance test results to match version 3 of VerySimpleXml
</commit_message>
<xml_diff>
--- a/PerformanceTests/XmlPerformanceTests.xlsx
+++ b/PerformanceTests/XmlPerformanceTests.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Development\Git\Neslib.Xml\PerformanceTests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23784E17-6A51-427F-AFE7-955B87F37573}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2201E416-E35A-4E1D-B844-0A4B844C4137}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" xr2:uid="{9C2BCDAD-6C83-4F4D-8B32-EE0B7AA119F2}"/>
   </bookViews>
@@ -342,7 +342,7 @@
                   <c:v>156428</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>245236</c:v>
+                  <c:v>202948</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>132152</c:v>
@@ -509,7 +509,7 @@
                   <c:v>278576</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>420572</c:v>
+                  <c:v>351184</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>219936</c:v>
@@ -999,7 +999,7 @@
                   <c:v>2308.0700000000002</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2379.1999999999998</c:v>
+                  <c:v>2030.4</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>93249.64</c:v>
@@ -1166,7 +1166,7 @@
                   <c:v>1491.38</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2074.59</c:v>
+                  <c:v>1681.5</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>91344.38</c:v>
@@ -1653,6 +1653,9 @@
                 <c:pt idx="2">
                   <c:v>235.8</c:v>
                 </c:pt>
+                <c:pt idx="3">
+                  <c:v>70.150000000000006</c:v>
+                </c:pt>
                 <c:pt idx="4">
                   <c:v>176.7</c:v>
                 </c:pt>
@@ -1816,6 +1819,9 @@
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>213.26</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>96.83</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>114.8</c:v>
@@ -2302,6 +2308,9 @@
                 <c:pt idx="2">
                   <c:v>8.91</c:v>
                 </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.78</c:v>
+                </c:pt>
                 <c:pt idx="4">
                   <c:v>7.55</c:v>
                 </c:pt>
@@ -2465,6 +2474,9 @@
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>9.3000000000000007</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8.36</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>7.45</c:v>
@@ -2952,7 +2964,7 @@
                   <c:v>313.29000000000002</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>220.47</c:v>
+                  <c:v>200.68</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>117.15</c:v>
@@ -3119,7 +3131,7 @@
                   <c:v>368.14</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>267.02999999999997</c:v>
+                  <c:v>246.02</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>135.57</c:v>
@@ -7016,7 +7028,7 @@
   <dimension ref="A1:N16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -7190,22 +7202,34 @@
         <v>12</v>
       </c>
       <c r="B9">
-        <v>245236</v>
+        <v>202948</v>
       </c>
       <c r="C9" s="3">
-        <v>2379.1999999999998</v>
+        <v>2030.4</v>
+      </c>
+      <c r="D9" s="3">
+        <v>70.150000000000006</v>
+      </c>
+      <c r="E9" s="3">
+        <v>5.78</v>
       </c>
       <c r="F9" s="3">
-        <v>220.47</v>
+        <v>200.68</v>
       </c>
       <c r="H9" s="5">
-        <v>420572</v>
+        <v>351184</v>
       </c>
       <c r="I9" s="3">
-        <v>2074.59</v>
+        <v>1681.5</v>
+      </c>
+      <c r="J9" s="3">
+        <v>96.83</v>
+      </c>
+      <c r="K9" s="3">
+        <v>8.36</v>
       </c>
       <c r="L9" s="3">
-        <v>267.02999999999997</v>
+        <v>246.02</v>
       </c>
       <c r="N9" t="s">
         <v>13</v>

</xml_diff>